<commit_message>
Altered loader to handle new file with 1 section removed
</commit_message>
<xml_diff>
--- a/usaspending_api/references/tests/data/data_transparency_crosswalk_test_file.xlsx
+++ b/usaspending_api/references/tests/data/data_transparency_crosswalk_test_file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tonysappe/dev/fedspendingtransparency/usaspending-api/usaspending_api/references/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4A11A1-70C2-1746-AA78-5441B4AE9024}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527634B0-C83D-304D-8816-F089F8A0C9B1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1220" windowWidth="29180" windowHeight="14960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'MDR, Broker, Python Crosswalk'!$A$2:$X$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Public!$A$2:$L$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Public!$A$2:$K$2</definedName>
     <definedName name="_Remove">'[1]Combined Master'!#REF!</definedName>
     <definedName name="hh">'[1]Combined Master'!#REF!</definedName>
     <definedName name="TEMP">'[1]Combined Master'!#REF!</definedName>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9151" uniqueCount="2671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9148" uniqueCount="2670">
   <si>
     <t>Located In</t>
   </si>
@@ -8503,9 +8503,6 @@
   </si>
   <si>
     <t>USA Spending Downloads</t>
-  </si>
-  <si>
-    <t>File</t>
   </si>
   <si>
     <t>FPDS Element</t>
@@ -8710,7 +8707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -8780,13 +8777,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -9229,44 +9220,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>2665</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="35" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="36" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="32"/>
+      <c r="I1" s="30"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="32"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="30"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
-      <c r="P1" s="38" t="s">
+      <c r="P1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="30" t="s">
+      <c r="Q1" s="30"/>
+      <c r="R1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="33" t="s">
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="32"/>
+      <c r="X1" s="30"/>
     </row>
     <row r="2" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -39015,11 +39006,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F6DD44-BF91-4939-BDC0-FF6405CFB13F}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -39027,79 +39018,72 @@
     <col min="1" max="1" width="21.83203125" style="23" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" style="23" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="23" customWidth="1"/>
-    <col min="4" max="4" width="18" style="23" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="23" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" style="23" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" style="23" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" style="23" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" style="23" customWidth="1"/>
-    <col min="12" max="12" width="18.83203125" style="23" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="23"/>
+    <col min="4" max="4" width="13.83203125" style="23" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="23" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="23" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="23" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" style="23" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" style="23" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" style="23" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" style="23" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
         <v>2665</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="25" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39" t="s">
+        <v>2668</v>
+      </c>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="38"/>
+    </row>
+    <row r="2" spans="1:11" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>2669</v>
       </c>
-      <c r="E1" s="41" t="s">
-        <v>2668</v>
-      </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="40"/>
-    </row>
-    <row r="2" spans="1:12" s="22" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>2670</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="28" t="s">
+      <c r="D2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="E2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="F2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="G2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="H2" s="26" t="s">
         <v>2666</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="I2" s="26" t="s">
         <v>2667</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="J2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="K2" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>432</v>
       </c>
@@ -39110,13 +39094,13 @@
         <v>432</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>54</v>
+        <v>434</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>434</v>
+        <v>56</v>
       </c>
       <c r="G3" s="24" t="s">
         <v>56</v>
@@ -39128,21 +39112,18 @@
         <v>56</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>56</v>
+        <v>435</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>435</v>
-      </c>
-      <c r="L3" s="24" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:L2" xr:uid="{341A6C6B-FA83-45CE-8FCE-61A83BD3F968}"/>
+  <autoFilter ref="A2:K2" xr:uid="{341A6C6B-FA83-45CE-8FCE-61A83BD3F968}"/>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>